<commit_message>
Final figure exports for report
</commit_message>
<xml_diff>
--- a/data/sam/MacroconsumptionEffect_HH_GEO.xlsx
+++ b/data/sam/MacroconsumptionEffect_HH_GEO.xlsx
@@ -410,8 +410,8 @@
   </sheetPr>
   <dimension ref="A1:AD119"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D100" activeCellId="0" sqref="D100"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AF107" activeCellId="0" sqref="AF107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4485,85 +4485,85 @@
         <v>14</v>
       </c>
       <c r="D90" s="4" t="n">
-        <v>0.025671</v>
+        <v>0.0377</v>
       </c>
       <c r="E90" s="4" t="n">
-        <v>0.017627</v>
+        <v>0.0299</v>
       </c>
       <c r="F90" s="4" t="n">
-        <v>0.027881</v>
+        <v>0.0378</v>
       </c>
       <c r="G90" s="4" t="n">
-        <v>0.036674</v>
+        <v>0.0471</v>
       </c>
       <c r="H90" s="4" t="n">
-        <v>0.021397</v>
+        <v>0.0228</v>
       </c>
       <c r="I90" s="4" t="n">
-        <v>0.024766</v>
+        <v>0.0325</v>
       </c>
       <c r="J90" s="4" t="n">
-        <v>0.009099</v>
+        <v>0.0097</v>
       </c>
       <c r="K90" s="4" t="n">
-        <v>0.003113</v>
+        <v>0.0067</v>
       </c>
       <c r="L90" s="4" t="n">
-        <v>0.005236</v>
+        <v>0.0074</v>
       </c>
       <c r="M90" s="4" t="n">
-        <v>0.019972</v>
+        <v>0.0238</v>
       </c>
       <c r="N90" s="4" t="n">
-        <v>-0.001737</v>
+        <v>-0.0044</v>
       </c>
       <c r="O90" s="4" t="n">
-        <v>0.002713</v>
+        <v>0.002</v>
       </c>
       <c r="P90" s="4" t="n">
-        <v>0.006288</v>
+        <v>0.004</v>
       </c>
       <c r="Q90" s="4" t="n">
-        <v>0.003264</v>
+        <v>0.0056</v>
       </c>
       <c r="R90" s="4" t="n">
-        <v>0.001404</v>
+        <v>0.0036</v>
       </c>
       <c r="S90" s="4" t="n">
-        <v>0.015676</v>
+        <v>0.0192</v>
       </c>
       <c r="T90" s="4" t="n">
-        <v>0.012683</v>
+        <v>0.0173</v>
       </c>
       <c r="U90" s="4" t="n">
-        <v>0.010032</v>
+        <v>0.0168</v>
       </c>
       <c r="V90" s="4" t="n">
-        <v>0.00873</v>
+        <v>0.0112</v>
       </c>
       <c r="W90" s="4" t="n">
-        <v>-0.000391</v>
+        <v>0.0022</v>
       </c>
       <c r="X90" s="4" t="n">
-        <v>-0.004102</v>
+        <v>-0.0051</v>
       </c>
       <c r="Y90" s="4" t="n">
-        <v>-0.011947</v>
+        <v>-0.0095</v>
       </c>
       <c r="Z90" s="4" t="n">
-        <v>-0.004458</v>
+        <v>-0.0042</v>
       </c>
       <c r="AA90" s="4" t="n">
-        <v>-0.009067</v>
+        <v>-0.0095</v>
       </c>
       <c r="AB90" s="4" t="n">
-        <v>-0.007359</v>
+        <v>-0.0067</v>
       </c>
       <c r="AC90" s="4" t="n">
-        <v>0.008446</v>
+        <v>0.0124</v>
       </c>
       <c r="AD90" s="4" t="n">
-        <v>0.022938</v>
+        <v>0.0239</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4574,85 +4574,85 @@
         <v>15</v>
       </c>
       <c r="D91" s="4" t="n">
-        <v>0.022744</v>
+        <v>0.0334</v>
       </c>
       <c r="E91" s="4" t="n">
-        <v>0.018166</v>
+        <v>0.0299</v>
       </c>
       <c r="F91" s="4" t="n">
-        <v>0.028213</v>
+        <v>0.0385</v>
       </c>
       <c r="G91" s="4" t="n">
-        <v>0.037774</v>
+        <v>0.0487</v>
       </c>
       <c r="H91" s="4" t="n">
-        <v>0.026007</v>
+        <v>0.0288</v>
       </c>
       <c r="I91" s="4" t="n">
-        <v>0.028734</v>
+        <v>0.0365</v>
       </c>
       <c r="J91" s="4" t="n">
-        <v>0.014884</v>
+        <v>0.0163</v>
       </c>
       <c r="K91" s="4" t="n">
-        <v>0.008194</v>
+        <v>0.0118</v>
       </c>
       <c r="L91" s="4" t="n">
-        <v>0.008712</v>
+        <v>0.0109</v>
       </c>
       <c r="M91" s="4" t="n">
-        <v>0.021066</v>
+        <v>0.0246</v>
       </c>
       <c r="N91" s="4" t="n">
-        <v>0.002899</v>
+        <v>0.0008</v>
       </c>
       <c r="O91" s="4" t="n">
-        <v>0.005456</v>
+        <v>0.0045</v>
       </c>
       <c r="P91" s="4" t="n">
-        <v>0.008088</v>
+        <v>0.0056</v>
       </c>
       <c r="Q91" s="4" t="n">
-        <v>0.005355</v>
+        <v>0.0068</v>
       </c>
       <c r="R91" s="4" t="n">
-        <v>0.003495</v>
+        <v>0.0051</v>
       </c>
       <c r="S91" s="4" t="n">
-        <v>0.015607</v>
+        <v>0.0186</v>
       </c>
       <c r="T91" s="4" t="n">
-        <v>0.014087</v>
+        <v>0.0183</v>
       </c>
       <c r="U91" s="4" t="n">
-        <v>0.012294</v>
+        <v>0.0186</v>
       </c>
       <c r="V91" s="4" t="n">
-        <v>0.011304</v>
+        <v>0.0141</v>
       </c>
       <c r="W91" s="4" t="n">
-        <v>0.003275</v>
+        <v>0.006</v>
       </c>
       <c r="X91" s="4" t="n">
-        <v>-0.000678</v>
+        <v>-0.0012</v>
       </c>
       <c r="Y91" s="4" t="n">
-        <v>-0.008263</v>
+        <v>-0.0062</v>
       </c>
       <c r="Z91" s="4" t="n">
-        <v>-0.002966</v>
+        <v>-0.0027</v>
       </c>
       <c r="AA91" s="4" t="n">
-        <v>-0.007098</v>
+        <v>-0.0076</v>
       </c>
       <c r="AB91" s="4" t="n">
-        <v>-0.006081</v>
+        <v>-0.0058</v>
       </c>
       <c r="AC91" s="4" t="n">
-        <v>0.007467</v>
+        <v>0.0107</v>
       </c>
       <c r="AD91" s="4" t="n">
-        <v>0.021535</v>
+        <v>0.0225</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4663,85 +4663,85 @@
         <v>16</v>
       </c>
       <c r="D92" s="4" t="n">
-        <v>0.020267</v>
+        <v>0.029</v>
       </c>
       <c r="E92" s="4" t="n">
-        <v>0.017535</v>
+        <v>0.0276</v>
       </c>
       <c r="F92" s="4" t="n">
-        <v>0.027086</v>
+        <v>0.0361</v>
       </c>
       <c r="G92" s="4" t="n">
-        <v>0.036517</v>
+        <v>0.046</v>
       </c>
       <c r="H92" s="4" t="n">
-        <v>0.026801</v>
+        <v>0.0291</v>
       </c>
       <c r="I92" s="4" t="n">
-        <v>0.029166</v>
+        <v>0.0355</v>
       </c>
       <c r="J92" s="4" t="n">
-        <v>0.01656</v>
+        <v>0.0174</v>
       </c>
       <c r="K92" s="4" t="n">
-        <v>0.009749</v>
+        <v>0.0123</v>
       </c>
       <c r="L92" s="4" t="n">
-        <v>0.009519</v>
+        <v>0.0109</v>
       </c>
       <c r="M92" s="4" t="n">
-        <v>0.020493</v>
+        <v>0.023</v>
       </c>
       <c r="N92" s="4" t="n">
-        <v>0.004464</v>
+        <v>0.002</v>
       </c>
       <c r="O92" s="4" t="n">
-        <v>0.006102</v>
+        <v>0.0045</v>
       </c>
       <c r="P92" s="4" t="n">
-        <v>0.008105</v>
+        <v>0.0052</v>
       </c>
       <c r="Q92" s="4" t="n">
-        <v>0.005676</v>
+        <v>0.0062</v>
       </c>
       <c r="R92" s="4" t="n">
-        <v>0.003761</v>
+        <v>0.0046</v>
       </c>
       <c r="S92" s="4" t="n">
-        <v>0.014735</v>
+        <v>0.0168</v>
       </c>
       <c r="T92" s="4" t="n">
-        <v>0.013936</v>
+        <v>0.0171</v>
       </c>
       <c r="U92" s="4" t="n">
-        <v>0.012595</v>
+        <v>0.0177</v>
       </c>
       <c r="V92" s="4" t="n">
-        <v>0.01173</v>
+        <v>0.0138</v>
       </c>
       <c r="W92" s="4" t="n">
-        <v>0.004488</v>
+        <v>0.0064</v>
       </c>
       <c r="X92" s="4" t="n">
-        <v>0.000291</v>
+        <v>-0.0007</v>
       </c>
       <c r="Y92" s="4" t="n">
-        <v>-0.0073</v>
+        <v>-0.0061</v>
       </c>
       <c r="Z92" s="4" t="n">
-        <v>-0.00315</v>
+        <v>-0.0035</v>
       </c>
       <c r="AA92" s="4" t="n">
-        <v>-0.007064</v>
+        <v>-0.0082</v>
       </c>
       <c r="AB92" s="4" t="n">
-        <v>-0.006458</v>
+        <v>-0.0069</v>
       </c>
       <c r="AC92" s="4" t="n">
-        <v>0.005983</v>
+        <v>0.0082</v>
       </c>
       <c r="AD92" s="4" t="n">
-        <v>0.019708</v>
+        <v>0.0198</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4752,85 +4752,85 @@
         <v>17</v>
       </c>
       <c r="D93" s="4" t="n">
-        <v>0.018566</v>
+        <v>0.0267</v>
       </c>
       <c r="E93" s="4" t="n">
-        <v>0.017492</v>
+        <v>0.0274</v>
       </c>
       <c r="F93" s="4" t="n">
-        <v>0.026784</v>
+        <v>0.036</v>
       </c>
       <c r="G93" s="4" t="n">
-        <v>0.036496</v>
+        <v>0.0463</v>
       </c>
       <c r="H93" s="4" t="n">
-        <v>0.028658</v>
+        <v>0.0319</v>
       </c>
       <c r="I93" s="4" t="n">
-        <v>0.030687</v>
+        <v>0.0372</v>
       </c>
       <c r="J93" s="4" t="n">
-        <v>0.019193</v>
+        <v>0.0206</v>
       </c>
       <c r="K93" s="4" t="n">
-        <v>0.012114</v>
+        <v>0.0148</v>
       </c>
       <c r="L93" s="4" t="n">
-        <v>0.01106</v>
+        <v>0.0126</v>
       </c>
       <c r="M93" s="4" t="n">
-        <v>0.020663</v>
+        <v>0.0232</v>
       </c>
       <c r="N93" s="4" t="n">
-        <v>0.006612</v>
+        <v>0.0046</v>
       </c>
       <c r="O93" s="4" t="n">
-        <v>0.007256</v>
+        <v>0.0057</v>
       </c>
       <c r="P93" s="4" t="n">
-        <v>0.008805</v>
+        <v>0.006</v>
       </c>
       <c r="Q93" s="4" t="n">
-        <v>0.00653</v>
+        <v>0.0067</v>
       </c>
       <c r="R93" s="4" t="n">
-        <v>0.004653</v>
+        <v>0.0053</v>
       </c>
       <c r="S93" s="4" t="n">
-        <v>0.014312</v>
+        <v>0.0162</v>
       </c>
       <c r="T93" s="4" t="n">
-        <v>0.014258</v>
+        <v>0.0174</v>
       </c>
       <c r="U93" s="4" t="n">
-        <v>0.013336</v>
+        <v>0.0184</v>
       </c>
       <c r="V93" s="4" t="n">
-        <v>0.012641</v>
+        <v>0.0151</v>
       </c>
       <c r="W93" s="4" t="n">
-        <v>0.00603</v>
+        <v>0.0082</v>
       </c>
       <c r="X93" s="4" t="n">
-        <v>0.001817</v>
+        <v>0.0013</v>
       </c>
       <c r="Y93" s="4" t="n">
-        <v>-0.005477</v>
+        <v>-0.0042</v>
       </c>
       <c r="Z93" s="4" t="n">
-        <v>-0.002541</v>
+        <v>-0.0026</v>
       </c>
       <c r="AA93" s="4" t="n">
-        <v>-0.006157</v>
+        <v>-0.007</v>
       </c>
       <c r="AB93" s="4" t="n">
-        <v>-0.005902</v>
+        <v>-0.0062</v>
       </c>
       <c r="AC93" s="4" t="n">
-        <v>0.00511</v>
+        <v>0.0072</v>
       </c>
       <c r="AD93" s="4" t="n">
-        <v>0.018314</v>
+        <v>0.0187</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4841,85 +4841,85 @@
         <v>18</v>
       </c>
       <c r="D94" s="4" t="n">
-        <v>0.01772</v>
+        <v>0.0234</v>
       </c>
       <c r="E94" s="4" t="n">
-        <v>0.018451</v>
+        <v>0.0262</v>
       </c>
       <c r="F94" s="4" t="n">
-        <v>0.028066</v>
+        <v>0.0354</v>
       </c>
       <c r="G94" s="4" t="n">
-        <v>0.038071</v>
+        <v>0.0456</v>
       </c>
       <c r="H94" s="4" t="n">
-        <v>0.031443</v>
+        <v>0.0328</v>
       </c>
       <c r="I94" s="4" t="n">
-        <v>0.033113</v>
+        <v>0.037</v>
       </c>
       <c r="J94" s="4" t="n">
-        <v>0.021736</v>
+        <v>0.0213</v>
       </c>
       <c r="K94" s="4" t="n">
-        <v>0.013897</v>
+        <v>0.0144</v>
       </c>
       <c r="L94" s="4" t="n">
-        <v>0.01196</v>
+        <v>0.0116</v>
       </c>
       <c r="M94" s="4" t="n">
-        <v>0.020866</v>
+        <v>0.0213</v>
       </c>
       <c r="N94" s="4" t="n">
-        <v>0.008069</v>
+        <v>0.0047</v>
       </c>
       <c r="O94" s="4" t="n">
-        <v>0.007811</v>
+        <v>0.0047</v>
       </c>
       <c r="P94" s="4" t="n">
-        <v>0.008597</v>
+        <v>0.0044</v>
       </c>
       <c r="Q94" s="4" t="n">
-        <v>0.006646</v>
+        <v>0.0052</v>
       </c>
       <c r="R94" s="4" t="n">
-        <v>0.004459</v>
+        <v>0.0036</v>
       </c>
       <c r="S94" s="4" t="n">
-        <v>0.013752</v>
+        <v>0.014</v>
       </c>
       <c r="T94" s="4" t="n">
-        <v>0.014493</v>
+        <v>0.0158</v>
       </c>
       <c r="U94" s="4" t="n">
-        <v>0.01406</v>
+        <v>0.017</v>
       </c>
       <c r="V94" s="4" t="n">
-        <v>0.013389</v>
+        <v>0.0141</v>
       </c>
       <c r="W94" s="4" t="n">
-        <v>0.007372</v>
+        <v>0.0077</v>
       </c>
       <c r="X94" s="4" t="n">
-        <v>0.002366</v>
+        <v>0.0003</v>
       </c>
       <c r="Y94" s="4" t="n">
-        <v>-0.0057</v>
+        <v>-0.0061</v>
       </c>
       <c r="Z94" s="4" t="n">
-        <v>-0.003789</v>
+        <v>-0.0055</v>
       </c>
       <c r="AA94" s="4" t="n">
-        <v>-0.007442</v>
+        <v>-0.0098</v>
       </c>
       <c r="AB94" s="4" t="n">
-        <v>-0.007655</v>
+        <v>-0.0095</v>
       </c>
       <c r="AC94" s="4" t="n">
-        <v>0.003119</v>
+        <v>0.0032</v>
       </c>
       <c r="AD94" s="4" t="n">
-        <v>0.016982</v>
+        <v>0.0152</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4930,85 +4930,85 @@
         <v>19</v>
       </c>
       <c r="D95" s="4" t="n">
-        <v>0.023783</v>
+        <v>0.035</v>
       </c>
       <c r="E95" s="4" t="n">
-        <v>0.018385</v>
+        <v>0.0304</v>
       </c>
       <c r="F95" s="4" t="n">
-        <v>0.028605</v>
+        <v>0.0389</v>
       </c>
       <c r="G95" s="4" t="n">
-        <v>0.038292</v>
+        <v>0.0492</v>
       </c>
       <c r="H95" s="4" t="n">
-        <v>0.025661</v>
+        <v>0.0282</v>
       </c>
       <c r="I95" s="4" t="n">
-        <v>0.028562</v>
+        <v>0.0364</v>
       </c>
       <c r="J95" s="4" t="n">
-        <v>0.01411</v>
+        <v>0.0154</v>
       </c>
       <c r="K95" s="4" t="n">
-        <v>0.007357</v>
+        <v>0.011</v>
       </c>
       <c r="L95" s="4" t="n">
-        <v>0.008096</v>
+        <v>0.0104</v>
       </c>
       <c r="M95" s="4" t="n">
-        <v>0.021047</v>
+        <v>0.0247</v>
       </c>
       <c r="N95" s="4" t="n">
-        <v>0.001901</v>
+        <v>-0.0004</v>
       </c>
       <c r="O95" s="4" t="n">
-        <v>0.004802</v>
+        <v>0.0039</v>
       </c>
       <c r="P95" s="4" t="n">
-        <v>0.007635</v>
+        <v>0.0052</v>
       </c>
       <c r="Q95" s="4" t="n">
-        <v>0.004793</v>
+        <v>0.0064</v>
       </c>
       <c r="R95" s="4" t="n">
-        <v>0.002878</v>
+        <v>0.0046</v>
       </c>
       <c r="S95" s="4" t="n">
-        <v>0.01546</v>
+        <v>0.0186</v>
       </c>
       <c r="T95" s="4" t="n">
-        <v>0.013611</v>
+        <v>0.0179</v>
       </c>
       <c r="U95" s="4" t="n">
-        <v>0.011573</v>
+        <v>0.018</v>
       </c>
       <c r="V95" s="4" t="n">
-        <v>0.010503</v>
+        <v>0.0133</v>
       </c>
       <c r="W95" s="4" t="n">
-        <v>0.00223</v>
+        <v>0.0049</v>
       </c>
       <c r="X95" s="4" t="n">
-        <v>-0.001729</v>
+        <v>-0.0023</v>
       </c>
       <c r="Y95" s="4" t="n">
-        <v>-0.009455</v>
+        <v>-0.0073</v>
       </c>
       <c r="Z95" s="4" t="n">
-        <v>-0.003787</v>
+        <v>-0.0035</v>
       </c>
       <c r="AA95" s="4" t="n">
-        <v>-0.008063</v>
+        <v>-0.0085</v>
       </c>
       <c r="AB95" s="4" t="n">
-        <v>-0.006938</v>
+        <v>-0.0065</v>
       </c>
       <c r="AC95" s="4" t="n">
-        <v>0.007053</v>
+        <v>0.0105</v>
       </c>
       <c r="AD95" s="4" t="n">
-        <v>0.021175</v>
+        <v>0.0221</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5019,85 +5019,85 @@
         <v>20</v>
       </c>
       <c r="D96" s="4" t="n">
-        <v>0.020644</v>
+        <v>0.0298</v>
       </c>
       <c r="E96" s="4" t="n">
-        <v>0.019267</v>
+        <v>0.0303</v>
       </c>
       <c r="F96" s="4" t="n">
-        <v>0.029398</v>
+        <v>0.0397</v>
       </c>
       <c r="G96" s="4" t="n">
-        <v>0.039913</v>
+        <v>0.0508</v>
       </c>
       <c r="H96" s="4" t="n">
-        <v>0.031164</v>
+        <v>0.0348</v>
       </c>
       <c r="I96" s="4" t="n">
-        <v>0.033259</v>
+        <v>0.0405</v>
       </c>
       <c r="J96" s="4" t="n">
-        <v>0.020694</v>
+        <v>0.0224</v>
       </c>
       <c r="K96" s="4" t="n">
-        <v>0.012983</v>
+        <v>0.016</v>
       </c>
       <c r="L96" s="4" t="n">
-        <v>0.011807</v>
+        <v>0.0136</v>
       </c>
       <c r="M96" s="4" t="n">
-        <v>0.022057</v>
+        <v>0.0249</v>
       </c>
       <c r="N96" s="4" t="n">
-        <v>0.006957</v>
+        <v>0.0049</v>
       </c>
       <c r="O96" s="4" t="n">
-        <v>0.007624</v>
+        <v>0.0061</v>
       </c>
       <c r="P96" s="4" t="n">
-        <v>0.009303</v>
+        <v>0.0064</v>
       </c>
       <c r="Q96" s="4" t="n">
-        <v>0.006861</v>
+        <v>0.0071</v>
       </c>
       <c r="R96" s="4" t="n">
-        <v>0.004876</v>
+        <v>0.0056</v>
       </c>
       <c r="S96" s="4" t="n">
-        <v>0.015026</v>
+        <v>0.0172</v>
       </c>
       <c r="T96" s="4" t="n">
-        <v>0.014943</v>
+        <v>0.0184</v>
       </c>
       <c r="U96" s="4" t="n">
-        <v>0.013936</v>
+        <v>0.0194</v>
       </c>
       <c r="V96" s="4" t="n">
-        <v>0.013187</v>
+        <v>0.016</v>
       </c>
       <c r="W96" s="4" t="n">
-        <v>0.006227</v>
+        <v>0.0087</v>
       </c>
       <c r="X96" s="4" t="n">
-        <v>0.001844</v>
+        <v>0.0015</v>
       </c>
       <c r="Y96" s="4" t="n">
-        <v>-0.005738</v>
+        <v>-0.0042</v>
       </c>
       <c r="Z96" s="4" t="n">
-        <v>-0.002684</v>
+        <v>-0.0026</v>
       </c>
       <c r="AA96" s="4" t="n">
-        <v>-0.006446</v>
+        <v>-0.0071</v>
       </c>
       <c r="AB96" s="4" t="n">
-        <v>-0.006153</v>
+        <v>-0.0063</v>
       </c>
       <c r="AC96" s="4" t="n">
-        <v>0.005277</v>
+        <v>0.0077</v>
       </c>
       <c r="AD96" s="4" t="n">
-        <v>0.018988</v>
+        <v>0.0196</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5108,85 +5108,85 @@
         <v>21</v>
       </c>
       <c r="D97" s="4" t="n">
-        <v>0.018054</v>
+        <v>0.0262</v>
       </c>
       <c r="E97" s="4" t="n">
-        <v>0.018542</v>
+        <v>0.0289</v>
       </c>
       <c r="F97" s="4" t="n">
-        <v>0.028081</v>
+        <v>0.0382</v>
       </c>
       <c r="G97" s="4" t="n">
-        <v>0.038657</v>
+        <v>0.0494</v>
       </c>
       <c r="H97" s="4" t="n">
-        <v>0.032265</v>
+        <v>0.0367</v>
       </c>
       <c r="I97" s="4" t="n">
-        <v>0.03396</v>
+        <v>0.041</v>
       </c>
       <c r="J97" s="4" t="n">
-        <v>0.022953</v>
+        <v>0.0252</v>
       </c>
       <c r="K97" s="4" t="n">
-        <v>0.015099</v>
+        <v>0.0181</v>
       </c>
       <c r="L97" s="4" t="n">
-        <v>0.013011</v>
+        <v>0.015</v>
       </c>
       <c r="M97" s="4" t="n">
-        <v>0.021519</v>
+        <v>0.0243</v>
       </c>
       <c r="N97" s="4" t="n">
-        <v>0.008892</v>
+        <v>0.0074</v>
       </c>
       <c r="O97" s="4" t="n">
-        <v>0.008436</v>
+        <v>0.007</v>
       </c>
       <c r="P97" s="4" t="n">
-        <v>0.009599</v>
+        <v>0.0068</v>
       </c>
       <c r="Q97" s="4" t="n">
-        <v>0.007381</v>
+        <v>0.0073</v>
       </c>
       <c r="R97" s="4" t="n">
-        <v>0.005456</v>
+        <v>0.006</v>
       </c>
       <c r="S97" s="4" t="n">
-        <v>0.013928</v>
+        <v>0.0159</v>
       </c>
       <c r="T97" s="4" t="n">
-        <v>0.014656</v>
+        <v>0.0179</v>
       </c>
       <c r="U97" s="4" t="n">
-        <v>0.014098</v>
+        <v>0.0194</v>
       </c>
       <c r="V97" s="4" t="n">
-        <v>0.013536</v>
+        <v>0.0167</v>
       </c>
       <c r="W97" s="4" t="n">
-        <v>0.00741</v>
+        <v>0.0103</v>
       </c>
       <c r="X97" s="4" t="n">
-        <v>0.003077</v>
+        <v>0.0033</v>
       </c>
       <c r="Y97" s="4" t="n">
-        <v>-0.004059</v>
+        <v>-0.0024</v>
       </c>
       <c r="Z97" s="4" t="n">
-        <v>-0.002448</v>
+        <v>-0.0019</v>
       </c>
       <c r="AA97" s="4" t="n">
-        <v>-0.005845</v>
+        <v>-0.006</v>
       </c>
       <c r="AB97" s="4" t="n">
-        <v>-0.00595</v>
+        <v>-0.0058</v>
       </c>
       <c r="AC97" s="4" t="n">
-        <v>0.003667</v>
+        <v>0.0061</v>
       </c>
       <c r="AD97" s="4" t="n">
-        <v>0.016481</v>
+        <v>0.0176</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5197,85 +5197,85 @@
         <v>22</v>
       </c>
       <c r="D98" s="4" t="n">
-        <v>0.017181</v>
+        <v>0.0244</v>
       </c>
       <c r="E98" s="4" t="n">
-        <v>0.018547</v>
+        <v>0.0282</v>
       </c>
       <c r="F98" s="4" t="n">
-        <v>0.028013</v>
+        <v>0.0375</v>
       </c>
       <c r="G98" s="4" t="n">
-        <v>0.038585</v>
+        <v>0.0487</v>
       </c>
       <c r="H98" s="4" t="n">
-        <v>0.033021</v>
+        <v>0.0371</v>
       </c>
       <c r="I98" s="4" t="n">
-        <v>0.034523</v>
+        <v>0.0408</v>
       </c>
       <c r="J98" s="4" t="n">
-        <v>0.023923</v>
+        <v>0.0257</v>
       </c>
       <c r="K98" s="4" t="n">
-        <v>0.015901</v>
+        <v>0.0183</v>
       </c>
       <c r="L98" s="4" t="n">
-        <v>0.01343</v>
+        <v>0.0149</v>
       </c>
       <c r="M98" s="4" t="n">
-        <v>0.02137</v>
+        <v>0.0235</v>
       </c>
       <c r="N98" s="4" t="n">
-        <v>0.009648</v>
+        <v>0.0079</v>
       </c>
       <c r="O98" s="4" t="n">
-        <v>0.008744</v>
+        <v>0.0069</v>
       </c>
       <c r="P98" s="4" t="n">
-        <v>0.009592</v>
+        <v>0.0065</v>
       </c>
       <c r="Q98" s="4" t="n">
-        <v>0.007521</v>
+        <v>0.0069</v>
       </c>
       <c r="R98" s="4" t="n">
-        <v>0.005541</v>
+        <v>0.0057</v>
       </c>
       <c r="S98" s="4" t="n">
-        <v>0.013574</v>
+        <v>0.015</v>
       </c>
       <c r="T98" s="4" t="n">
-        <v>0.01468</v>
+        <v>0.0174</v>
       </c>
       <c r="U98" s="4" t="n">
-        <v>0.014364</v>
+        <v>0.019</v>
       </c>
       <c r="V98" s="4" t="n">
-        <v>0.013851</v>
+        <v>0.0166</v>
       </c>
       <c r="W98" s="4" t="n">
-        <v>0.00806</v>
+        <v>0.0104</v>
       </c>
       <c r="X98" s="4" t="n">
-        <v>0.00354</v>
+        <v>0.0035</v>
       </c>
       <c r="Y98" s="4" t="n">
-        <v>-0.003689</v>
+        <v>-0.0025</v>
       </c>
       <c r="Z98" s="4" t="n">
-        <v>-0.002609</v>
+        <v>-0.0024</v>
       </c>
       <c r="AA98" s="4" t="n">
-        <v>-0.005929</v>
+        <v>-0.0065</v>
       </c>
       <c r="AB98" s="4" t="n">
-        <v>-0.006231</v>
+        <v>-0.0065</v>
       </c>
       <c r="AC98" s="4" t="n">
-        <v>0.002974</v>
+        <v>0.0049</v>
       </c>
       <c r="AD98" s="4" t="n">
-        <v>0.015805</v>
+        <v>0.0164</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5286,85 +5286,85 @@
         <v>23</v>
       </c>
       <c r="D99" s="4" t="n">
-        <v>0.015983</v>
+        <v>0.0215</v>
       </c>
       <c r="E99" s="4" t="n">
-        <v>0.018385</v>
+        <v>0.0264</v>
       </c>
       <c r="F99" s="4" t="n">
-        <v>0.027733</v>
+        <v>0.0358</v>
       </c>
       <c r="G99" s="4" t="n">
-        <v>0.038124</v>
+        <v>0.0465</v>
       </c>
       <c r="H99" s="4" t="n">
-        <v>0.033488</v>
+        <v>0.0363</v>
       </c>
       <c r="I99" s="4" t="n">
-        <v>0.034776</v>
+        <v>0.0394</v>
       </c>
       <c r="J99" s="4" t="n">
-        <v>0.024602</v>
+        <v>0.0252</v>
       </c>
       <c r="K99" s="4" t="n">
-        <v>0.016403</v>
+        <v>0.0175</v>
       </c>
       <c r="L99" s="4" t="n">
-        <v>0.013518</v>
+        <v>0.0138</v>
       </c>
       <c r="M99" s="4" t="n">
-        <v>0.020886</v>
+        <v>0.0218</v>
       </c>
       <c r="N99" s="4" t="n">
-        <v>0.010169</v>
+        <v>0.0076</v>
       </c>
       <c r="O99" s="4" t="n">
-        <v>0.008793</v>
+        <v>0.0061</v>
       </c>
       <c r="P99" s="4" t="n">
-        <v>0.009214</v>
+        <v>0.0054</v>
       </c>
       <c r="Q99" s="4" t="n">
-        <v>0.007386</v>
+        <v>0.0059</v>
       </c>
       <c r="R99" s="4" t="n">
-        <v>0.00528</v>
+        <v>0.0046</v>
       </c>
       <c r="S99" s="4" t="n">
-        <v>0.012969</v>
+        <v>0.0135</v>
       </c>
       <c r="T99" s="4" t="n">
-        <v>0.014514</v>
+        <v>0.0162</v>
       </c>
       <c r="U99" s="4" t="n">
-        <v>0.014494</v>
+        <v>0.0179</v>
       </c>
       <c r="V99" s="4" t="n">
-        <v>0.014005</v>
+        <v>0.0158</v>
       </c>
       <c r="W99" s="4" t="n">
-        <v>0.008647</v>
+        <v>0.01</v>
       </c>
       <c r="X99" s="4" t="n">
-        <v>0.00376</v>
+        <v>0.0029</v>
       </c>
       <c r="Y99" s="4" t="n">
-        <v>-0.00378</v>
+        <v>-0.0034</v>
       </c>
       <c r="Z99" s="4" t="n">
-        <v>-0.003281</v>
+        <v>-0.0039</v>
       </c>
       <c r="AA99" s="4" t="n">
-        <v>-0.006572</v>
+        <v>-0.0079</v>
       </c>
       <c r="AB99" s="4" t="n">
-        <v>-0.007118</v>
+        <v>-0.0081</v>
       </c>
       <c r="AC99" s="4" t="n">
-        <v>0.001836</v>
+        <v>0.0026</v>
       </c>
       <c r="AD99" s="4" t="n">
-        <v>0.014864</v>
+        <v>0.0143</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5375,85 +5375,85 @@
         <v>14</v>
       </c>
       <c r="D100" s="4" t="n">
-        <v>0.004773</v>
+        <v>0.0173</v>
       </c>
       <c r="E100" s="4" t="n">
-        <v>0.017428</v>
+        <v>0.0267</v>
       </c>
       <c r="F100" s="4" t="n">
-        <v>0.043411</v>
+        <v>0.0651</v>
       </c>
       <c r="G100" s="4" t="n">
-        <v>0.036833</v>
+        <v>0.0544</v>
       </c>
       <c r="H100" s="4" t="n">
-        <v>0.036514</v>
+        <v>0.0516</v>
       </c>
       <c r="I100" s="4" t="n">
-        <v>0.016801</v>
+        <v>0.0253</v>
       </c>
       <c r="J100" s="4" t="n">
-        <v>0.00888</v>
+        <v>0.0156</v>
       </c>
       <c r="K100" s="4" t="n">
-        <v>-0.001416</v>
+        <v>0.0005</v>
       </c>
       <c r="L100" s="4" t="n">
-        <v>0.009891</v>
+        <v>0.0162</v>
       </c>
       <c r="M100" s="4" t="n">
-        <v>0.008421</v>
+        <v>0.0116</v>
       </c>
       <c r="N100" s="4" t="n">
-        <v>0.025783</v>
+        <v>0.033</v>
       </c>
       <c r="O100" s="4" t="n">
-        <v>0.035988</v>
+        <v>0.0445</v>
       </c>
       <c r="P100" s="4" t="n">
-        <v>0.04248</v>
+        <v>0.0554</v>
       </c>
       <c r="Q100" s="4" t="n">
-        <v>0.04264</v>
+        <v>0.053</v>
       </c>
       <c r="R100" s="4" t="n">
-        <v>0.054175</v>
+        <v>0.0621</v>
       </c>
       <c r="S100" s="4" t="n">
-        <v>0.042047</v>
+        <v>0.0467</v>
       </c>
       <c r="T100" s="4" t="n">
-        <v>0.040504</v>
+        <v>0.0458</v>
       </c>
       <c r="U100" s="4" t="n">
-        <v>0.018782</v>
+        <v>0.0209</v>
       </c>
       <c r="V100" s="4" t="n">
-        <v>0.030018</v>
+        <v>0.0384</v>
       </c>
       <c r="W100" s="4" t="n">
-        <v>0.032589</v>
+        <v>0.0369</v>
       </c>
       <c r="X100" s="4" t="n">
-        <v>0.031369</v>
+        <v>0.0397</v>
       </c>
       <c r="Y100" s="4" t="n">
-        <v>0.036801</v>
+        <v>0.0484</v>
       </c>
       <c r="Z100" s="4" t="n">
-        <v>0.049105</v>
+        <v>0.0541</v>
       </c>
       <c r="AA100" s="4" t="n">
-        <v>0.042013</v>
+        <v>0.0451</v>
       </c>
       <c r="AB100" s="4" t="n">
-        <v>0.036984</v>
+        <v>0.0452</v>
       </c>
       <c r="AC100" s="4" t="n">
-        <v>0.058505</v>
+        <v>0.0647</v>
       </c>
       <c r="AD100" s="4" t="n">
-        <v>0.043014</v>
+        <v>0.0486</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5464,85 +5464,85 @@
         <v>15</v>
       </c>
       <c r="D101" s="4" t="n">
-        <v>0.004385</v>
+        <v>0.0154</v>
       </c>
       <c r="E101" s="4" t="n">
-        <v>0.015877</v>
+        <v>0.0251</v>
       </c>
       <c r="F101" s="4" t="n">
-        <v>0.040472</v>
+        <v>0.0611</v>
       </c>
       <c r="G101" s="4" t="n">
-        <v>0.038511</v>
+        <v>0.0568</v>
       </c>
       <c r="H101" s="4" t="n">
-        <v>0.040096</v>
+        <v>0.0565</v>
       </c>
       <c r="I101" s="4" t="n">
-        <v>0.023649</v>
+        <v>0.0341</v>
       </c>
       <c r="J101" s="4" t="n">
-        <v>0.015417</v>
+        <v>0.0235</v>
       </c>
       <c r="K101" s="4" t="n">
-        <v>0.004731</v>
+        <v>0.0079</v>
       </c>
       <c r="L101" s="4" t="n">
-        <v>0.012811</v>
+        <v>0.0193</v>
       </c>
       <c r="M101" s="4" t="n">
-        <v>0.011328</v>
+        <v>0.015</v>
       </c>
       <c r="N101" s="4" t="n">
-        <v>0.026326</v>
+        <v>0.0333</v>
       </c>
       <c r="O101" s="4" t="n">
-        <v>0.036772</v>
+        <v>0.0452</v>
       </c>
       <c r="P101" s="4" t="n">
-        <v>0.044368</v>
+        <v>0.0569</v>
       </c>
       <c r="Q101" s="4" t="n">
-        <v>0.046216</v>
+        <v>0.057</v>
       </c>
       <c r="R101" s="4" t="n">
-        <v>0.057439</v>
+        <v>0.0662</v>
       </c>
       <c r="S101" s="4" t="n">
-        <v>0.0484</v>
+        <v>0.0541</v>
       </c>
       <c r="T101" s="4" t="n">
-        <v>0.047005</v>
+        <v>0.0528</v>
       </c>
       <c r="U101" s="4" t="n">
-        <v>0.02765</v>
+        <v>0.0305</v>
       </c>
       <c r="V101" s="4" t="n">
-        <v>0.035434</v>
+        <v>0.0435</v>
       </c>
       <c r="W101" s="4" t="n">
-        <v>0.037272</v>
+        <v>0.042</v>
       </c>
       <c r="X101" s="4" t="n">
-        <v>0.036217</v>
+        <v>0.0443</v>
       </c>
       <c r="Y101" s="4" t="n">
-        <v>0.040891</v>
+        <v>0.0521</v>
       </c>
       <c r="Z101" s="4" t="n">
-        <v>0.052169</v>
+        <v>0.0579</v>
       </c>
       <c r="AA101" s="4" t="n">
-        <v>0.047279</v>
+        <v>0.051</v>
       </c>
       <c r="AB101" s="4" t="n">
-        <v>0.043164</v>
+        <v>0.051</v>
       </c>
       <c r="AC101" s="4" t="n">
-        <v>0.061956</v>
+        <v>0.0682</v>
       </c>
       <c r="AD101" s="4" t="n">
-        <v>0.050075</v>
+        <v>0.0557</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5553,85 +5553,85 @@
         <v>16</v>
       </c>
       <c r="D102" s="4" t="n">
-        <v>0.003532</v>
+        <v>0.0127</v>
       </c>
       <c r="E102" s="4" t="n">
-        <v>0.014297</v>
+        <v>0.0223</v>
       </c>
       <c r="F102" s="4" t="n">
-        <v>0.038059</v>
+        <v>0.0562</v>
       </c>
       <c r="G102" s="4" t="n">
-        <v>0.038376</v>
+        <v>0.0549</v>
       </c>
       <c r="H102" s="4" t="n">
-        <v>0.040942</v>
+        <v>0.0558</v>
       </c>
       <c r="I102" s="4" t="n">
-        <v>0.026627</v>
+        <v>0.0361</v>
       </c>
       <c r="J102" s="4" t="n">
-        <v>0.018452</v>
+        <v>0.0257</v>
       </c>
       <c r="K102" s="4" t="n">
-        <v>0.007715</v>
+        <v>0.0105</v>
       </c>
       <c r="L102" s="4" t="n">
-        <v>0.014018</v>
+        <v>0.0195</v>
       </c>
       <c r="M102" s="4" t="n">
-        <v>0.012451</v>
+        <v>0.0155</v>
       </c>
       <c r="N102" s="4" t="n">
-        <v>0.025947</v>
+        <v>0.0318</v>
       </c>
       <c r="O102" s="4" t="n">
-        <v>0.036123</v>
+        <v>0.0433</v>
       </c>
       <c r="P102" s="4" t="n">
-        <v>0.043708</v>
+        <v>0.0546</v>
       </c>
       <c r="Q102" s="4" t="n">
-        <v>0.046099</v>
+        <v>0.0557</v>
       </c>
       <c r="R102" s="4" t="n">
-        <v>0.05642</v>
+        <v>0.0642</v>
       </c>
       <c r="S102" s="4" t="n">
-        <v>0.049089</v>
+        <v>0.0541</v>
       </c>
       <c r="T102" s="4" t="n">
-        <v>0.047655</v>
+        <v>0.0526</v>
       </c>
       <c r="U102" s="4" t="n">
-        <v>0.030131</v>
+        <v>0.0324</v>
       </c>
       <c r="V102" s="4" t="n">
-        <v>0.03598</v>
+        <v>0.0427</v>
       </c>
       <c r="W102" s="4" t="n">
-        <v>0.037587</v>
+        <v>0.0414</v>
       </c>
       <c r="X102" s="4" t="n">
-        <v>0.036499</v>
+        <v>0.0431</v>
       </c>
       <c r="Y102" s="4" t="n">
-        <v>0.040693</v>
+        <v>0.05</v>
       </c>
       <c r="Z102" s="4" t="n">
-        <v>0.051085</v>
+        <v>0.0557</v>
       </c>
       <c r="AA102" s="4" t="n">
-        <v>0.047517</v>
+        <v>0.0502</v>
       </c>
       <c r="AB102" s="4" t="n">
-        <v>0.044011</v>
+        <v>0.0502</v>
       </c>
       <c r="AC102" s="4" t="n">
-        <v>0.060822</v>
+        <v>0.0657</v>
       </c>
       <c r="AD102" s="4" t="n">
-        <v>0.051161</v>
+        <v>0.0555</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5642,85 +5642,85 @@
         <v>17</v>
       </c>
       <c r="D103" s="4" t="n">
-        <v>0.003361</v>
+        <v>0.0119</v>
       </c>
       <c r="E103" s="4" t="n">
-        <v>0.013335</v>
+        <v>0.0213</v>
       </c>
       <c r="F103" s="4" t="n">
-        <v>0.035883</v>
+        <v>0.0534</v>
       </c>
       <c r="G103" s="4" t="n">
-        <v>0.038483</v>
+        <v>0.0554</v>
       </c>
       <c r="H103" s="4" t="n">
-        <v>0.041939</v>
+        <v>0.0575</v>
       </c>
       <c r="I103" s="4" t="n">
-        <v>0.029465</v>
+        <v>0.04</v>
       </c>
       <c r="J103" s="4" t="n">
-        <v>0.021295</v>
+        <v>0.0293</v>
       </c>
       <c r="K103" s="4" t="n">
-        <v>0.010572</v>
+        <v>0.0141</v>
       </c>
       <c r="L103" s="4" t="n">
-        <v>0.015183</v>
+        <v>0.0208</v>
       </c>
       <c r="M103" s="4" t="n">
-        <v>0.013644</v>
+        <v>0.0171</v>
       </c>
       <c r="N103" s="4" t="n">
-        <v>0.025774</v>
+        <v>0.0317</v>
       </c>
       <c r="O103" s="4" t="n">
-        <v>0.035933</v>
+        <v>0.0432</v>
       </c>
       <c r="P103" s="4" t="n">
-        <v>0.044014</v>
+        <v>0.0548</v>
       </c>
       <c r="Q103" s="4" t="n">
-        <v>0.047258</v>
+        <v>0.0572</v>
       </c>
       <c r="R103" s="4" t="n">
-        <v>0.05741</v>
+        <v>0.0658</v>
       </c>
       <c r="S103" s="4" t="n">
-        <v>0.051743</v>
+        <v>0.0574</v>
       </c>
       <c r="T103" s="4" t="n">
-        <v>0.05048</v>
+        <v>0.0559</v>
       </c>
       <c r="U103" s="4" t="n">
-        <v>0.034375</v>
+        <v>0.0373</v>
       </c>
       <c r="V103" s="4" t="n">
-        <v>0.03848</v>
+        <v>0.0452</v>
       </c>
       <c r="W103" s="4" t="n">
-        <v>0.039659</v>
+        <v>0.044</v>
       </c>
       <c r="X103" s="4" t="n">
-        <v>0.03875</v>
+        <v>0.0455</v>
       </c>
       <c r="Y103" s="4" t="n">
-        <v>0.042499</v>
+        <v>0.052</v>
       </c>
       <c r="Z103" s="4" t="n">
-        <v>0.052265</v>
+        <v>0.0577</v>
       </c>
       <c r="AA103" s="4" t="n">
-        <v>0.049838</v>
+        <v>0.0532</v>
       </c>
       <c r="AB103" s="4" t="n">
-        <v>0.046855</v>
+        <v>0.0532</v>
       </c>
       <c r="AC103" s="4" t="n">
-        <v>0.062155</v>
+        <v>0.0674</v>
       </c>
       <c r="AD103" s="4" t="n">
-        <v>0.054435</v>
+        <v>0.0591</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5731,85 +5731,85 @@
         <v>18</v>
       </c>
       <c r="D104" s="4" t="n">
-        <v>0.002076</v>
+        <v>0.0086</v>
       </c>
       <c r="E104" s="4" t="n">
-        <v>0.012738</v>
+        <v>0.0191</v>
       </c>
       <c r="F104" s="4" t="n">
-        <v>0.037807</v>
+        <v>0.0529</v>
       </c>
       <c r="G104" s="4" t="n">
-        <v>0.042741</v>
+        <v>0.0572</v>
       </c>
       <c r="H104" s="4" t="n">
-        <v>0.047517</v>
+        <v>0.0605</v>
       </c>
       <c r="I104" s="4" t="n">
-        <v>0.036026</v>
+        <v>0.0443</v>
       </c>
       <c r="J104" s="4" t="n">
-        <v>0.026949</v>
+        <v>0.0328</v>
       </c>
       <c r="K104" s="4" t="n">
-        <v>0.014923</v>
+        <v>0.0168</v>
       </c>
       <c r="L104" s="4" t="n">
-        <v>0.017863</v>
+        <v>0.0214</v>
       </c>
       <c r="M104" s="4" t="n">
-        <v>0.0159</v>
+        <v>0.0177</v>
       </c>
       <c r="N104" s="4" t="n">
-        <v>0.027212</v>
+        <v>0.031</v>
       </c>
       <c r="O104" s="4" t="n">
-        <v>0.037536</v>
+        <v>0.0424</v>
       </c>
       <c r="P104" s="4" t="n">
-        <v>0.045659</v>
+        <v>0.0538</v>
       </c>
       <c r="Q104" s="4" t="n">
-        <v>0.049386</v>
+        <v>0.0572</v>
       </c>
       <c r="R104" s="4" t="n">
-        <v>0.058445</v>
+        <v>0.0648</v>
       </c>
       <c r="S104" s="4" t="n">
-        <v>0.054226</v>
+        <v>0.0581</v>
       </c>
       <c r="T104" s="4" t="n">
-        <v>0.05259</v>
+        <v>0.0561</v>
       </c>
       <c r="U104" s="4" t="n">
-        <v>0.037752</v>
+        <v>0.039</v>
       </c>
       <c r="V104" s="4" t="n">
-        <v>0.03976</v>
+        <v>0.044</v>
       </c>
       <c r="W104" s="4" t="n">
-        <v>0.040964</v>
+        <v>0.043</v>
       </c>
       <c r="X104" s="4" t="n">
-        <v>0.039697</v>
+        <v>0.0436</v>
       </c>
       <c r="Y104" s="4" t="n">
-        <v>0.043133</v>
+        <v>0.0492</v>
       </c>
       <c r="Z104" s="4" t="n">
-        <v>0.052237</v>
+        <v>0.0548</v>
       </c>
       <c r="AA104" s="4" t="n">
-        <v>0.051358</v>
+        <v>0.052</v>
       </c>
       <c r="AB104" s="4" t="n">
-        <v>0.048969</v>
+        <v>0.0521</v>
       </c>
       <c r="AC104" s="4" t="n">
-        <v>0.062532</v>
+        <v>0.0648</v>
       </c>
       <c r="AD104" s="4" t="n">
-        <v>0.057143</v>
+        <v>0.059</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5820,85 +5820,85 @@
         <v>19</v>
       </c>
       <c r="D105" s="4" t="n">
-        <v>0.00451</v>
+        <v>0.0161</v>
       </c>
       <c r="E105" s="4" t="n">
-        <v>0.016461</v>
+        <v>0.0259</v>
       </c>
       <c r="F105" s="4" t="n">
-        <v>0.041746</v>
+        <v>0.0628</v>
       </c>
       <c r="G105" s="4" t="n">
-        <v>0.039055</v>
+        <v>0.0575</v>
       </c>
       <c r="H105" s="4" t="n">
-        <v>0.040333</v>
+        <v>0.0566</v>
       </c>
       <c r="I105" s="4" t="n">
-        <v>0.023007</v>
+        <v>0.0332</v>
       </c>
       <c r="J105" s="4" t="n">
-        <v>0.014668</v>
+        <v>0.0226</v>
       </c>
       <c r="K105" s="4" t="n">
-        <v>0.003823</v>
+        <v>0.0068</v>
       </c>
       <c r="L105" s="4" t="n">
-        <v>0.012583</v>
+        <v>0.0192</v>
       </c>
       <c r="M105" s="4" t="n">
-        <v>0.011017</v>
+        <v>0.0147</v>
       </c>
       <c r="N105" s="4" t="n">
-        <v>0.02668</v>
+        <v>0.0338</v>
       </c>
       <c r="O105" s="4" t="n">
-        <v>0.037191</v>
+        <v>0.0457</v>
       </c>
       <c r="P105" s="4" t="n">
-        <v>0.044507</v>
+        <v>0.0572</v>
       </c>
       <c r="Q105" s="4" t="n">
-        <v>0.0459</v>
+        <v>0.0566</v>
       </c>
       <c r="R105" s="4" t="n">
-        <v>0.057179</v>
+        <v>0.0657</v>
       </c>
       <c r="S105" s="4" t="n">
-        <v>0.047414</v>
+        <v>0.0528</v>
       </c>
       <c r="T105" s="4" t="n">
-        <v>0.045895</v>
+        <v>0.0516</v>
       </c>
       <c r="U105" s="4" t="n">
-        <v>0.025997</v>
+        <v>0.0287</v>
       </c>
       <c r="V105" s="4" t="n">
-        <v>0.034493</v>
+        <v>0.0426</v>
       </c>
       <c r="W105" s="4" t="n">
-        <v>0.036441</v>
+        <v>0.0411</v>
       </c>
       <c r="X105" s="4" t="n">
-        <v>0.035377</v>
+        <v>0.0435</v>
       </c>
       <c r="Y105" s="4" t="n">
-        <v>0.040143</v>
+        <v>0.0514</v>
       </c>
       <c r="Z105" s="4" t="n">
-        <v>0.05161</v>
+        <v>0.0572</v>
       </c>
       <c r="AA105" s="4" t="n">
-        <v>0.046288</v>
+        <v>0.0498</v>
       </c>
       <c r="AB105" s="4" t="n">
-        <v>0.042006</v>
+        <v>0.0498</v>
       </c>
       <c r="AC105" s="4" t="n">
-        <v>0.061298</v>
+        <v>0.0674</v>
       </c>
       <c r="AD105" s="4" t="n">
-        <v>0.048788</v>
+        <v>0.0543</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5909,85 +5909,85 @@
         <v>20</v>
       </c>
       <c r="D106" s="4" t="n">
-        <v>0.003771</v>
+        <v>0.0134</v>
       </c>
       <c r="E106" s="4" t="n">
-        <v>0.01474</v>
+        <v>0.0237</v>
       </c>
       <c r="F106" s="4" t="n">
-        <v>0.039365</v>
+        <v>0.0588</v>
       </c>
       <c r="G106" s="4" t="n">
-        <v>0.042004</v>
+        <v>0.0606</v>
       </c>
       <c r="H106" s="4" t="n">
-        <v>0.045564</v>
+        <v>0.0627</v>
       </c>
       <c r="I106" s="4" t="n">
-        <v>0.031812</v>
+        <v>0.0434</v>
       </c>
       <c r="J106" s="4" t="n">
-        <v>0.022875</v>
+        <v>0.0317</v>
       </c>
       <c r="K106" s="4" t="n">
-        <v>0.011278</v>
+        <v>0.0153</v>
       </c>
       <c r="L106" s="4" t="n">
-        <v>0.016228</v>
+        <v>0.0225</v>
       </c>
       <c r="M106" s="4" t="n">
-        <v>0.014539</v>
+        <v>0.0183</v>
       </c>
       <c r="N106" s="4" t="n">
-        <v>0.027471</v>
+        <v>0.0339</v>
       </c>
       <c r="O106" s="4" t="n">
-        <v>0.038216</v>
+        <v>0.0461</v>
       </c>
       <c r="P106" s="4" t="n">
-        <v>0.046726</v>
+        <v>0.0584</v>
       </c>
       <c r="Q106" s="4" t="n">
-        <v>0.050077</v>
+        <v>0.0607</v>
       </c>
       <c r="R106" s="4" t="n">
-        <v>0.060794</v>
+        <v>0.0698</v>
       </c>
       <c r="S106" s="4" t="n">
-        <v>0.054683</v>
+        <v>0.0608</v>
       </c>
       <c r="T106" s="4" t="n">
-        <v>0.053324</v>
+        <v>0.0592</v>
       </c>
       <c r="U106" s="4" t="n">
-        <v>0.036298</v>
+        <v>0.0395</v>
       </c>
       <c r="V106" s="4" t="n">
-        <v>0.040627</v>
+        <v>0.0479</v>
       </c>
       <c r="W106" s="4" t="n">
-        <v>0.041803</v>
+        <v>0.0465</v>
       </c>
       <c r="X106" s="4" t="n">
-        <v>0.040856</v>
+        <v>0.0482</v>
       </c>
       <c r="Y106" s="4" t="n">
-        <v>0.044747</v>
+        <v>0.055</v>
       </c>
       <c r="Z106" s="4" t="n">
-        <v>0.054939</v>
+        <v>0.0609</v>
       </c>
       <c r="AA106" s="4" t="n">
-        <v>0.052346</v>
+        <v>0.0561</v>
       </c>
       <c r="AB106" s="4" t="n">
-        <v>0.04921</v>
+        <v>0.0561</v>
       </c>
       <c r="AC106" s="4" t="n">
-        <v>0.065212</v>
+        <v>0.0709</v>
       </c>
       <c r="AD106" s="4" t="n">
-        <v>0.057107</v>
+        <v>0.0622</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5998,85 +5998,85 @@
         <v>21</v>
       </c>
       <c r="D107" s="4" t="n">
-        <v>0.003374</v>
+        <v>0.0119</v>
       </c>
       <c r="E107" s="4" t="n">
-        <v>0.013135</v>
+        <v>0.0218</v>
       </c>
       <c r="F107" s="4" t="n">
-        <v>0.035739</v>
+        <v>0.0538</v>
       </c>
       <c r="G107" s="4" t="n">
-        <v>0.040984</v>
+        <v>0.0593</v>
       </c>
       <c r="H107" s="4" t="n">
-        <v>0.045509</v>
+        <v>0.0627</v>
       </c>
       <c r="I107" s="4" t="n">
-        <v>0.03421</v>
+        <v>0.0465</v>
       </c>
       <c r="J107" s="4" t="n">
-        <v>0.025522</v>
+        <v>0.0349</v>
       </c>
       <c r="K107" s="4" t="n">
-        <v>0.014206</v>
+        <v>0.019</v>
       </c>
       <c r="L107" s="4" t="n">
-        <v>0.017168</v>
+        <v>0.0234</v>
       </c>
       <c r="M107" s="4" t="n">
-        <v>0.015519</v>
+        <v>0.0197</v>
       </c>
       <c r="N107" s="4" t="n">
-        <v>0.026684</v>
+        <v>0.033</v>
       </c>
       <c r="O107" s="4" t="n">
-        <v>0.037157</v>
+        <v>0.0448</v>
       </c>
       <c r="P107" s="4" t="n">
-        <v>0.045987</v>
+        <v>0.0572</v>
       </c>
       <c r="Q107" s="4" t="n">
-        <v>0.050204</v>
+        <v>0.0609</v>
       </c>
       <c r="R107" s="4" t="n">
-        <v>0.060539</v>
+        <v>0.0699</v>
       </c>
       <c r="S107" s="4" t="n">
-        <v>0.056412</v>
+        <v>0.0632</v>
       </c>
       <c r="T107" s="4" t="n">
-        <v>0.055334</v>
+        <v>0.0617</v>
       </c>
       <c r="U107" s="4" t="n">
-        <v>0.040282</v>
+        <v>0.0441</v>
       </c>
       <c r="V107" s="4" t="n">
-        <v>0.042641</v>
+        <v>0.0499</v>
       </c>
       <c r="W107" s="4" t="n">
-        <v>0.043338</v>
+        <v>0.0486</v>
       </c>
       <c r="X107" s="4" t="n">
-        <v>0.042659</v>
+        <v>0.0502</v>
       </c>
       <c r="Y107" s="4" t="n">
-        <v>0.045987</v>
+        <v>0.0564</v>
       </c>
       <c r="Z107" s="4" t="n">
-        <v>0.055311</v>
+        <v>0.0622</v>
       </c>
       <c r="AA107" s="4" t="n">
-        <v>0.054043</v>
+        <v>0.0587</v>
       </c>
       <c r="AB107" s="4" t="n">
-        <v>0.051583</v>
+        <v>0.0587</v>
       </c>
       <c r="AC107" s="4" t="n">
-        <v>0.065705</v>
+        <v>0.0719</v>
       </c>
       <c r="AD107" s="4" t="n">
-        <v>0.059895</v>
+        <v>0.0654</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6087,85 +6087,85 @@
         <v>22</v>
       </c>
       <c r="D108" s="4" t="n">
-        <v>0.002931</v>
+        <v>0.0107</v>
       </c>
       <c r="E108" s="4" t="n">
-        <v>0.01257</v>
+        <v>0.0206</v>
       </c>
       <c r="F108" s="4" t="n">
-        <v>0.035334</v>
+        <v>0.0524</v>
       </c>
       <c r="G108" s="4" t="n">
-        <v>0.041636</v>
+        <v>0.0592</v>
       </c>
       <c r="H108" s="4" t="n">
-        <v>0.046673</v>
+        <v>0.0632</v>
       </c>
       <c r="I108" s="4" t="n">
-        <v>0.03618</v>
+        <v>0.0479</v>
       </c>
       <c r="J108" s="4" t="n">
-        <v>0.027347</v>
+        <v>0.0362</v>
       </c>
       <c r="K108" s="4" t="n">
-        <v>0.015812</v>
+        <v>0.0202</v>
       </c>
       <c r="L108" s="4" t="n">
-        <v>0.017928</v>
+        <v>0.0236</v>
       </c>
       <c r="M108" s="4" t="n">
-        <v>0.016199</v>
+        <v>0.0199</v>
       </c>
       <c r="N108" s="4" t="n">
-        <v>0.026734</v>
+        <v>0.0324</v>
       </c>
       <c r="O108" s="4" t="n">
-        <v>0.037156</v>
+        <v>0.0441</v>
       </c>
       <c r="P108" s="4" t="n">
-        <v>0.046068</v>
+        <v>0.0564</v>
       </c>
       <c r="Q108" s="4" t="n">
-        <v>0.05061</v>
+        <v>0.0607</v>
       </c>
       <c r="R108" s="4" t="n">
-        <v>0.06057</v>
+        <v>0.0695</v>
       </c>
       <c r="S108" s="4" t="n">
-        <v>0.05725</v>
+        <v>0.0637</v>
       </c>
       <c r="T108" s="4" t="n">
-        <v>0.056151</v>
+        <v>0.062</v>
       </c>
       <c r="U108" s="4" t="n">
-        <v>0.041848</v>
+        <v>0.0454</v>
       </c>
       <c r="V108" s="4" t="n">
-        <v>0.043255</v>
+        <v>0.0498</v>
       </c>
       <c r="W108" s="4" t="n">
-        <v>0.04388</v>
+        <v>0.0486</v>
       </c>
       <c r="X108" s="4" t="n">
-        <v>0.043147</v>
+        <v>0.05</v>
       </c>
       <c r="Y108" s="4" t="n">
-        <v>0.046301</v>
+        <v>0.0558</v>
       </c>
       <c r="Z108" s="4" t="n">
-        <v>0.055285</v>
+        <v>0.0615</v>
       </c>
       <c r="AA108" s="4" t="n">
-        <v>0.054695</v>
+        <v>0.0587</v>
       </c>
       <c r="AB108" s="4" t="n">
-        <v>0.052523</v>
+        <v>0.0588</v>
       </c>
       <c r="AC108" s="4" t="n">
-        <v>0.065825</v>
+        <v>0.0713</v>
       </c>
       <c r="AD108" s="4" t="n">
-        <v>0.061071</v>
+        <v>0.0659</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6176,85 +6176,85 @@
         <v>23</v>
       </c>
       <c r="D109" s="4" t="n">
-        <v>0.002034</v>
+        <v>0.0082</v>
       </c>
       <c r="E109" s="4" t="n">
-        <v>0.011724</v>
+        <v>0.0185</v>
       </c>
       <c r="F109" s="4" t="n">
-        <v>0.035204</v>
+        <v>0.0502</v>
       </c>
       <c r="G109" s="4" t="n">
-        <v>0.042666</v>
+        <v>0.0582</v>
       </c>
       <c r="H109" s="4" t="n">
-        <v>0.048357</v>
+        <v>0.0628</v>
       </c>
       <c r="I109" s="4" t="n">
-        <v>0.038807</v>
+        <v>0.0488</v>
       </c>
       <c r="J109" s="4" t="n">
-        <v>0.029756</v>
+        <v>0.037</v>
       </c>
       <c r="K109" s="4" t="n">
-        <v>0.017827</v>
+        <v>0.0211</v>
       </c>
       <c r="L109" s="4" t="n">
-        <v>0.018955</v>
+        <v>0.0232</v>
       </c>
       <c r="M109" s="4" t="n">
-        <v>0.017046</v>
+        <v>0.0197</v>
       </c>
       <c r="N109" s="4" t="n">
-        <v>0.026884</v>
+        <v>0.0312</v>
       </c>
       <c r="O109" s="4" t="n">
-        <v>0.03717</v>
+        <v>0.0426</v>
       </c>
       <c r="P109" s="4" t="n">
-        <v>0.045952</v>
+        <v>0.0545</v>
       </c>
       <c r="Q109" s="4" t="n">
-        <v>0.050727</v>
+        <v>0.0594</v>
       </c>
       <c r="R109" s="4" t="n">
-        <v>0.059921</v>
+        <v>0.0675</v>
       </c>
       <c r="S109" s="4" t="n">
-        <v>0.057524</v>
+        <v>0.0628</v>
       </c>
       <c r="T109" s="4" t="n">
-        <v>0.056305</v>
+        <v>0.061</v>
       </c>
       <c r="U109" s="4" t="n">
-        <v>0.043008</v>
+        <v>0.0455</v>
       </c>
       <c r="V109" s="4" t="n">
-        <v>0.043259</v>
+        <v>0.0483</v>
       </c>
       <c r="W109" s="4" t="n">
-        <v>0.043928</v>
+        <v>0.0473</v>
       </c>
       <c r="X109" s="4" t="n">
-        <v>0.043035</v>
+        <v>0.0482</v>
       </c>
       <c r="Y109" s="4" t="n">
-        <v>0.046004</v>
+        <v>0.0535</v>
       </c>
       <c r="Z109" s="4" t="n">
-        <v>0.054513</v>
+        <v>0.0591</v>
       </c>
       <c r="AA109" s="4" t="n">
-        <v>0.054816</v>
+        <v>0.0573</v>
       </c>
       <c r="AB109" s="4" t="n">
-        <v>0.053033</v>
+        <v>0.0575</v>
       </c>
       <c r="AC109" s="4" t="n">
-        <v>0.065253</v>
+        <v>0.069</v>
       </c>
       <c r="AD109" s="4" t="n">
-        <v>0.061853</v>
+        <v>0.0651</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>